<commit_message>
minor change to column headings
</commit_message>
<xml_diff>
--- a/SSD_rawdata.xlsx
+++ b/SSD_rawdata.xlsx
@@ -74,7 +74,7 @@
     <t xml:space="preserve">dose.mg.L.master.converted.reported</t>
   </si>
   <si>
-    <t xml:space="preserve">Dose_Volume_Aligned</t>
+    <t xml:space="preserve">Dose_Volume_Aligned_particles_L</t>
   </si>
   <si>
     <t xml:space="preserve">Acute_Chronic_AF</t>
@@ -638,7 +638,7 @@
     <t xml:space="preserve">Polylactic Acid</t>
   </si>
   <si>
-    <t xml:space="preserve">Dose_SurfaceArea_Aligned</t>
+    <t xml:space="preserve">Dose_SurfaceArea_Aligned_particles_L</t>
   </si>
 </sst>
 </file>

</xml_diff>